<commit_message>
Answered all question up to 3
</commit_message>
<xml_diff>
--- a/03 - Interactive Viz/amstat_all.xlsx
+++ b/03 - Interactive Viz/amstat_all.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="29120" windowHeight="9120"/>
+    <workbookView xWindow="4480" yWindow="3160" windowWidth="29120" windowHeight="13520"/>
   </bookViews>
   <sheets>
     <sheet name="2.1 Taux de chômage" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>Suisse alémanique</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Espace Mittelland</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
     <t>Soleure</t>
   </si>
   <si>
-    <t>2.6</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>Zurich</t>
   </si>
   <si>
-    <t>3.3</t>
-  </si>
-  <si>
     <t>Ostschweiz</t>
   </si>
   <si>
@@ -116,9 +107,6 @@
     <t>Grisons</t>
   </si>
   <si>
-    <t>1.1</t>
-  </si>
-  <si>
     <t>Thurgovie</t>
   </si>
   <si>
@@ -131,9 +119,6 @@
     <t>Uri</t>
   </si>
   <si>
-    <t>0.6</t>
-  </si>
-  <si>
     <t>Schwyz</t>
   </si>
   <si>
@@ -170,9 +155,6 @@
     <t>Genève</t>
   </si>
   <si>
-    <t>5.2</t>
-  </si>
-  <si>
     <t>Fribourg</t>
   </si>
   <si>
@@ -197,9 +179,6 @@
     <t>Tessin</t>
   </si>
   <si>
-    <t>3.1</t>
-  </si>
-  <si>
     <t>ling_reg</t>
   </si>
   <si>
@@ -212,13 +191,16 @@
     <t>rate</t>
   </si>
   <si>
-    <t>unempl_c</t>
-  </si>
-  <si>
-    <t>jobseek_c</t>
-  </si>
-  <si>
-    <t>empl_jobseek_c</t>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>5.3</t>
   </si>
 </sst>
 </file>
@@ -537,8 +519,8 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -553,25 +535,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -579,598 +552,442 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1">
-        <v>13658</v>
-      </c>
-      <c r="F2" s="1">
-        <v>18385</v>
-      </c>
-      <c r="G2" s="1">
-        <v>4727</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3801</v>
-      </c>
-      <c r="F3" s="1">
-        <v>6628</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2827</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3455</v>
-      </c>
-      <c r="F4" s="1">
-        <v>5168</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1713</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4082</v>
-      </c>
-      <c r="F5" s="1">
-        <v>5540</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1458</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1">
-        <v>10684</v>
-      </c>
-      <c r="F6" s="1">
-        <v>15145</v>
-      </c>
-      <c r="G6" s="1">
-        <v>4461</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1">
-        <v>27225</v>
-      </c>
-      <c r="F7" s="1">
-        <v>34156</v>
-      </c>
-      <c r="G7" s="1">
-        <v>6931</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1">
-        <v>416</v>
-      </c>
-      <c r="F8" s="1">
-        <v>713</v>
-      </c>
-      <c r="G8" s="1">
-        <v>297</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
       <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1286</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2328</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1042</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="1">
-        <v>523</v>
-      </c>
-      <c r="F10" s="1">
-        <v>866</v>
-      </c>
-      <c r="G10" s="1">
-        <v>343</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="1">
-        <v>62</v>
-      </c>
-      <c r="F11" s="1">
-        <v>102</v>
-      </c>
-      <c r="G11" s="1">
-        <v>40</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="1">
-        <v>6127</v>
-      </c>
-      <c r="F12" s="1">
-        <v>10363</v>
-      </c>
-      <c r="G12" s="1">
-        <v>4236</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1166</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2590</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1424</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>3058</v>
-      </c>
-      <c r="F14" s="1">
-        <v>5618</v>
-      </c>
-      <c r="G14" s="1">
-        <v>2560</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3885</v>
-      </c>
-      <c r="F15" s="1">
-        <v>6756</v>
-      </c>
-      <c r="G15" s="1">
-        <v>2871</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="1">
-        <v>112</v>
-      </c>
-      <c r="F16" s="1">
-        <v>257</v>
-      </c>
-      <c r="G16" s="1">
-        <v>145</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1455</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2229</v>
-      </c>
-      <c r="G17" s="1">
-        <v>774</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
-        <v>36</v>
-      </c>
       <c r="D18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="1">
-        <v>153</v>
-      </c>
-      <c r="F18" s="1">
-        <v>319</v>
-      </c>
-      <c r="G18" s="1">
-        <v>166</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="1">
-        <v>248</v>
-      </c>
-      <c r="F19" s="1">
-        <v>436</v>
-      </c>
-      <c r="G19" s="1">
-        <v>188</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1543</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2615</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1072</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="1">
-        <v>17155</v>
-      </c>
-      <c r="F21" s="1">
-        <v>24649</v>
-      </c>
-      <c r="G21" s="1">
-        <v>7494</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="1">
-        <v>4816</v>
-      </c>
-      <c r="F22" s="1">
-        <v>8027</v>
-      </c>
-      <c r="G22" s="1">
-        <v>3211</v>
-      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
-      </c>
       <c r="D23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="1">
-        <v>12234</v>
-      </c>
-      <c r="F23" s="1">
-        <v>15497</v>
-      </c>
-      <c r="G23" s="1">
-        <v>3263</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="1">
-        <v>4466</v>
-      </c>
-      <c r="F24" s="1">
-        <v>7837</v>
-      </c>
-      <c r="G24" s="1">
-        <v>3371</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="1">
-        <v>4738</v>
-      </c>
-      <c r="F25" s="1">
-        <v>6350</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1612</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1619</v>
-      </c>
-      <c r="F26" s="1">
-        <v>2375</v>
-      </c>
-      <c r="G26" s="1">
-        <v>756</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="1">
-        <v>5202</v>
-      </c>
-      <c r="F27" s="1">
-        <v>8675</v>
-      </c>
-      <c r="G27" s="1">
-        <v>3473</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>